<commit_message>
Update Schwall_Gayathri_Timesheet_september_2021 - Copy - Copy.xlsx
</commit_message>
<xml_diff>
--- a/Gayathri/Timesheet/Schwall_Gayathri_Timesheet_september_2021 - Copy - Copy.xlsx
+++ b/Gayathri/Timesheet/Schwall_Gayathri_Timesheet_september_2021 - Copy - Copy.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E44A42B-54B9-4F0A-958A-50B972BC2635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9070A993-4AEA-42EA-9402-91D3615D09D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>SlNo</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>interview question</t>
+  </si>
+  <si>
+    <t>spring,spring boot</t>
   </si>
 </sst>
 </file>
@@ -566,7 +569,7 @@
   <dimension ref="B1:F145"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -733,18 +736,38 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="2"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="3"/>
+      <c r="B12" s="2">
+        <v>7</v>
+      </c>
+      <c r="C12" s="10">
+        <v>44446</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="3">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="2"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="3"/>
+      <c r="B13" s="2">
+        <v>8</v>
+      </c>
+      <c r="C13" s="10">
+        <v>44447</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>

</xml_diff>